<commit_message>
uploaded data deleted. some of them
</commit_message>
<xml_diff>
--- a/web/templates/add-unit-template.xlsx
+++ b/web/templates/add-unit-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yii2_stok_barang\web\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webvimark_stok_barang\web\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1362A-3FE3-4284-9F2C-A39EAA15E6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AB0AE4-0717-4D43-B44B-CDB1CFD3979B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{732D6342-8BE7-4639-A766-7FF72DF9C6DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id_wh</t>
   </si>
@@ -47,28 +47,19 @@
     <t>comment</t>
   </si>
   <si>
-    <t>warehouse's id</t>
-  </si>
-  <si>
-    <t>will autogenerate if empty</t>
-  </si>
-  <si>
-    <t>comment about unit. Will autogenerate if empty</t>
-  </si>
-  <si>
-    <t>example below</t>
-  </si>
-  <si>
-    <t>empty serial number. Serial number will auto generate</t>
-  </si>
-  <si>
-    <t>HGPS-123</t>
-  </si>
-  <si>
-    <t>serial number not empty. Will not autogenerate</t>
-  </si>
-  <si>
-    <t>Comment content here</t>
+    <t>HGST-00001</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>id_wh needs to be filled with id of the selected warehouse</t>
+  </si>
+  <si>
+    <t>serial number will auto generate if empty</t>
+  </si>
+  <si>
+    <t>comment will auto generate if empty</t>
   </si>
 </sst>
 </file>
@@ -440,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685BB158-DD99-4891-9DA2-7E37A48E1785}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +444,7 @@
     <col min="3" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,47 +455,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>